<commit_message>
Update Zeiterfassung & Projektplan
</commit_message>
<xml_diff>
--- a/Arbeitsdokumente/Projektplan GANTT.xlsx
+++ b/Arbeitsdokumente/Projektplan GANTT.xlsx
@@ -8,24 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan Samardzic\Documents\GitHub\PS_InfoEng\Arbeitsdokumente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC1E746-2057-4910-AA2A-C4AE85D2BF38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0ABB814-6710-4469-91D5-D183E0C55B6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="46">
   <si>
     <t>Projektbeginn:</t>
   </si>
@@ -478,7 +483,14 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="40">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1116,13 +1128,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:EG70"/>
+  <dimension ref="A1:EG71"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="DE36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="DS39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
+      <selection pane="bottomRight" activeCell="DW64" sqref="DW64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8766,13 +8778,13 @@
     </row>
     <row r="55" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B55" s="10">
-        <v>43486</v>
+        <v>43500</v>
       </c>
       <c r="C55" s="10">
-        <v>43501</v>
+        <v>43507</v>
       </c>
       <c r="D55" s="12"/>
       <c r="E55" s="12"/>
@@ -8911,13 +8923,13 @@
     </row>
     <row r="56" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B56" s="10">
+        <v>43486</v>
+      </c>
+      <c r="C56" s="10">
         <v>43501</v>
-      </c>
-      <c r="C56" s="10">
-        <v>43508</v>
       </c>
       <c r="D56" s="12"/>
       <c r="E56" s="12"/>
@@ -9056,13 +9068,13 @@
     </row>
     <row r="57" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B57" s="10">
-        <v>43490</v>
+        <v>43501</v>
       </c>
       <c r="C57" s="10">
-        <v>43509</v>
+        <v>43508</v>
       </c>
       <c r="D57" s="12"/>
       <c r="E57" s="12"/>
@@ -9201,13 +9213,13 @@
     </row>
     <row r="58" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B58" s="10">
-        <v>43509</v>
+        <v>43490</v>
       </c>
       <c r="C58" s="10">
-        <v>43509</v>
+        <v>43508</v>
       </c>
       <c r="D58" s="12"/>
       <c r="E58" s="12"/>
@@ -9345,9 +9357,15 @@
       <c r="EG58" s="12"/>
     </row>
     <row r="59" spans="1:137" x14ac:dyDescent="0.25">
-      <c r="A59" s="9"/>
-      <c r="B59" s="10"/>
-      <c r="C59" s="10"/>
+      <c r="A59" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B59" s="10">
+        <v>43508</v>
+      </c>
+      <c r="C59" s="10">
+        <v>43508</v>
+      </c>
       <c r="D59" s="12"/>
       <c r="E59" s="12"/>
       <c r="F59" s="12"/>
@@ -11012,194 +11030,338 @@
       <c r="EF70" s="12"/>
       <c r="EG70" s="12"/>
     </row>
+    <row r="71" spans="1:137" x14ac:dyDescent="0.25">
+      <c r="A71" s="9"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
+      <c r="H71" s="12"/>
+      <c r="I71" s="12"/>
+      <c r="J71" s="12"/>
+      <c r="K71" s="12"/>
+      <c r="L71" s="12"/>
+      <c r="M71" s="12"/>
+      <c r="N71" s="12"/>
+      <c r="O71" s="12"/>
+      <c r="P71" s="12"/>
+      <c r="Q71" s="12"/>
+      <c r="R71" s="12"/>
+      <c r="S71" s="12"/>
+      <c r="T71" s="12"/>
+      <c r="U71" s="12"/>
+      <c r="V71" s="12"/>
+      <c r="W71" s="12"/>
+      <c r="X71" s="12"/>
+      <c r="Y71" s="12"/>
+      <c r="Z71" s="12"/>
+      <c r="AA71" s="12"/>
+      <c r="AB71" s="12"/>
+      <c r="AC71" s="12"/>
+      <c r="AD71" s="12"/>
+      <c r="AE71" s="12"/>
+      <c r="AF71" s="12"/>
+      <c r="AG71" s="12"/>
+      <c r="AH71" s="12"/>
+      <c r="AI71" s="12"/>
+      <c r="AJ71" s="12"/>
+      <c r="AK71" s="12"/>
+      <c r="AL71" s="12"/>
+      <c r="AM71" s="12"/>
+      <c r="AN71" s="12"/>
+      <c r="AO71" s="12"/>
+      <c r="AP71" s="12"/>
+      <c r="AQ71" s="12"/>
+      <c r="AR71" s="12"/>
+      <c r="AS71" s="12"/>
+      <c r="AT71" s="12"/>
+      <c r="AU71" s="12"/>
+      <c r="AV71" s="12"/>
+      <c r="AW71" s="12"/>
+      <c r="AX71" s="12"/>
+      <c r="AY71" s="12"/>
+      <c r="AZ71" s="12"/>
+      <c r="BA71" s="12"/>
+      <c r="BB71" s="12"/>
+      <c r="BC71" s="12"/>
+      <c r="BD71" s="12"/>
+      <c r="BE71" s="12"/>
+      <c r="BF71" s="12"/>
+      <c r="BG71" s="12"/>
+      <c r="BH71" s="12"/>
+      <c r="BI71" s="12"/>
+      <c r="BJ71" s="12"/>
+      <c r="BK71" s="12"/>
+      <c r="BL71" s="12"/>
+      <c r="BM71" s="12"/>
+      <c r="BN71" s="12"/>
+      <c r="BO71" s="12"/>
+      <c r="BP71" s="12"/>
+      <c r="BQ71" s="12"/>
+      <c r="BR71" s="12"/>
+      <c r="BS71" s="12"/>
+      <c r="BT71" s="12"/>
+      <c r="BU71" s="12"/>
+      <c r="BV71" s="12"/>
+      <c r="BW71" s="12"/>
+      <c r="BX71" s="12"/>
+      <c r="BY71" s="12"/>
+      <c r="BZ71" s="12"/>
+      <c r="CA71" s="12"/>
+      <c r="CB71" s="12"/>
+      <c r="CC71" s="12"/>
+      <c r="CD71" s="12"/>
+      <c r="CE71" s="12"/>
+      <c r="CF71" s="12"/>
+      <c r="CG71" s="12"/>
+      <c r="CH71" s="12"/>
+      <c r="CI71" s="12"/>
+      <c r="CJ71" s="12"/>
+      <c r="CK71" s="12"/>
+      <c r="CL71" s="12"/>
+      <c r="CM71" s="12"/>
+      <c r="CN71" s="12"/>
+      <c r="CO71" s="12"/>
+      <c r="CP71" s="12"/>
+      <c r="CQ71" s="12"/>
+      <c r="CR71" s="12"/>
+      <c r="CS71" s="12"/>
+      <c r="CT71" s="12"/>
+      <c r="CU71" s="12"/>
+      <c r="CV71" s="12"/>
+      <c r="CW71" s="12"/>
+      <c r="CX71" s="12"/>
+      <c r="CY71" s="12"/>
+      <c r="CZ71" s="12"/>
+      <c r="DA71" s="12"/>
+      <c r="DB71" s="12"/>
+      <c r="DC71" s="12"/>
+      <c r="DD71" s="12"/>
+      <c r="DE71" s="12"/>
+      <c r="DF71" s="12"/>
+      <c r="DG71" s="12"/>
+      <c r="DH71" s="12"/>
+      <c r="DI71" s="12"/>
+      <c r="DJ71" s="12"/>
+      <c r="DK71" s="12"/>
+      <c r="DL71" s="12"/>
+      <c r="DM71" s="12"/>
+      <c r="DN71" s="12"/>
+      <c r="DO71" s="12"/>
+      <c r="DP71" s="12"/>
+      <c r="DQ71" s="12"/>
+      <c r="DR71" s="12"/>
+      <c r="DS71" s="12"/>
+      <c r="DT71" s="12"/>
+      <c r="DU71" s="12"/>
+      <c r="DV71" s="12"/>
+      <c r="DW71" s="12"/>
+      <c r="DX71" s="12"/>
+      <c r="DY71" s="12"/>
+      <c r="DZ71" s="12"/>
+      <c r="EA71" s="12"/>
+      <c r="EB71" s="12"/>
+      <c r="EC71" s="12"/>
+      <c r="ED71" s="12"/>
+      <c r="EE71" s="12"/>
+      <c r="EF71" s="12"/>
+      <c r="EG71" s="12"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D5:EG30 D32:EG32 D34:EG40 D41:CL44 CP41:EG44 CM42:CO44 D45:EG70">
-    <cfRule type="expression" dxfId="38" priority="62">
+  <conditionalFormatting sqref="D5:EG30 D32:EG32 D34:EG40 D41:CL44 CP41:EG44 CM42:CO44 D45:EG71">
+    <cfRule type="expression" dxfId="39" priority="62">
       <formula>D$5=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="63">
+    <cfRule type="expression" dxfId="38" priority="63">
       <formula>D$5=$C$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:AH4">
-    <cfRule type="expression" dxfId="36" priority="61">
+    <cfRule type="expression" dxfId="37" priority="61">
       <formula>D$5=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7:EG23 D26:EG30 D23:CL29 CP23:EG29 D32:CL32 CP32:EG32 D34:CL70 CP34:EG70">
-    <cfRule type="expression" dxfId="35" priority="69">
+  <conditionalFormatting sqref="D7:EG23 D26:EG30 D23:CL29 CP23:EG29 D32:CL32 CP32:EG32 D34:CL71 CP34:EG71">
+    <cfRule type="expression" dxfId="36" priority="69">
       <formula>AND(D$5&gt;=$B7,D$5&lt;=$C7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:AY6">
-    <cfRule type="expression" dxfId="34" priority="55">
+    <cfRule type="expression" dxfId="35" priority="55">
       <formula>AND(D$5&gt;=$B6,D$5&lt;=$C6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA6:EG6">
-    <cfRule type="expression" dxfId="33" priority="54">
+    <cfRule type="expression" dxfId="34" priority="54">
       <formula>AND(BA$5&gt;=$B6,BA$5&lt;=$C6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30:CI30 CQ30:EG30">
-    <cfRule type="expression" dxfId="32" priority="72">
+    <cfRule type="expression" dxfId="33" priority="72">
       <formula>AND(D$5&gt;=#REF!,D$5&lt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D21:EG23 BA26:CI30 CQ26:EG30 D23:CL29 BA20:EG29 D32:EG32 D34:EG40 D41:CL44 CP41:EG44 CM42:CO44 D45:EG70">
-    <cfRule type="expression" dxfId="31" priority="76">
+  <conditionalFormatting sqref="D21:EG23 BA26:CI30 CQ26:EG30 D23:CL29 BA20:EG29 D32:EG32 D34:EG40 D41:CL44 CP41:EG44 CM42:CO44 D45:EG71">
+    <cfRule type="expression" dxfId="32" priority="76">
       <formula>AND(D$5&gt;=#REF!,D$5&lt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CM22:CO22">
-    <cfRule type="expression" dxfId="30" priority="130">
+    <cfRule type="expression" dxfId="31" priority="130">
       <formula>AND(CM$5&gt;=$B28,CM$5&lt;=$C28)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:CI27 CQ27:EG27">
-    <cfRule type="expression" dxfId="29" priority="152">
+    <cfRule type="expression" dxfId="30" priority="152">
       <formula>AND(D$5&gt;=#REF!,D$5&lt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:CI26 CQ26:EG26 CM25:CO25">
-    <cfRule type="expression" dxfId="28" priority="156">
+    <cfRule type="expression" dxfId="29" priority="156">
       <formula>AND(D$5&gt;=#REF!,D$5&lt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CM23:CO23">
-    <cfRule type="expression" dxfId="27" priority="197">
+    <cfRule type="expression" dxfId="28" priority="197">
       <formula>AND(CM$5&gt;=$B30,CM$5&lt;=$C30)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20:EG20">
-    <cfRule type="expression" dxfId="26" priority="201">
+    <cfRule type="expression" dxfId="27" priority="201">
       <formula>AND(D$5&gt;=$B30,D$5&lt;=$C30)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CM23:CO29 CM35:CO40 CM42:CO43 CM45:CO70">
-    <cfRule type="expression" dxfId="25" priority="207">
+  <conditionalFormatting sqref="CM23:CO29 CM35:CO40 CM42:CO43 CM45:CO52 CM55:CO71">
+    <cfRule type="expression" dxfId="26" priority="207">
       <formula>AND(CM$5&gt;=$B24,CM$5&lt;=$C24)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ26:CP30">
-    <cfRule type="expression" dxfId="24" priority="35">
+    <cfRule type="expression" dxfId="25" priority="35">
       <formula>AND(CJ$5&gt;=#REF!,CJ$5&lt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25:CL25 CP25:EG25">
-    <cfRule type="expression" dxfId="23" priority="296">
+    <cfRule type="expression" dxfId="24" priority="296">
       <formula>AND(D$5&gt;=$B32,D$5&lt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CM23:CO24 CM27:CO29 CM32:CO32 CM35:CO40 CM42:CO43 CM45:CO70">
-    <cfRule type="expression" dxfId="22" priority="299">
+  <conditionalFormatting sqref="CM23:CO24 CM27:CO29 CM32:CO32 CM35:CO40 CM42:CO43 CM45:CO45 CM55:CO71">
+    <cfRule type="expression" dxfId="23" priority="299">
       <formula>AND(CM$5&gt;=$B31,CM$5&lt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ30:CP30">
-    <cfRule type="expression" dxfId="21" priority="324">
+    <cfRule type="expression" dxfId="22" priority="324">
       <formula>AND(CJ$5&gt;=$B37,CJ$5&lt;=$C35)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ29:CP29">
-    <cfRule type="expression" dxfId="20" priority="329">
+    <cfRule type="expression" dxfId="21" priority="329">
       <formula>AND(CJ$5&gt;=$B37,CJ$5&lt;=$C35)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ26:CP26">
-    <cfRule type="expression" dxfId="19" priority="331">
+    <cfRule type="expression" dxfId="20" priority="331">
       <formula>AND(CJ$5&gt;=$B37,CJ$5&lt;=$C35)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28:CI28 CQ28:EG28">
-    <cfRule type="expression" dxfId="18" priority="320">
+    <cfRule type="expression" dxfId="19" priority="320">
       <formula>AND(D$5&gt;=$B34,D$5&lt;=$C32)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:EG31">
-    <cfRule type="expression" dxfId="17" priority="20">
+    <cfRule type="expression" dxfId="18" priority="20">
       <formula>D$5=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="21">
+    <cfRule type="expression" dxfId="17" priority="21">
       <formula>D$5=$C$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:EG31">
-    <cfRule type="expression" dxfId="15" priority="22">
+    <cfRule type="expression" dxfId="16" priority="22">
       <formula>AND(D$5&gt;=$B31,D$5&lt;=$C31)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CM25:CO25">
-    <cfRule type="expression" dxfId="14" priority="335">
+    <cfRule type="expression" dxfId="15" priority="335">
       <formula>AND(CM$5&gt;=$B34,CM$5&lt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CM26:CO26">
-    <cfRule type="expression" dxfId="13" priority="336">
+    <cfRule type="expression" dxfId="14" priority="336">
       <formula>AND(CM$5&gt;=#REF!,CM$5&lt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CM25:CO25">
-    <cfRule type="expression" dxfId="12" priority="337">
+    <cfRule type="expression" dxfId="13" priority="337">
       <formula>AND(CM$5&gt;=$B34,CM$5&lt;=$C32)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29:CI29 CQ29:EG29">
-    <cfRule type="expression" dxfId="11" priority="338">
+    <cfRule type="expression" dxfId="12" priority="338">
       <formula>AND(D$5&gt;=#REF!,D$5&lt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30:CI30 CQ30:EG30">
-    <cfRule type="expression" dxfId="10" priority="340">
+    <cfRule type="expression" dxfId="11" priority="340">
       <formula>AND(D$5&gt;=#REF!,D$5&lt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ28:CP28">
-    <cfRule type="expression" dxfId="9" priority="344">
+    <cfRule type="expression" dxfId="10" priority="344">
       <formula>AND(CJ$5&gt;=$B36,CJ$5&lt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CM34:CO34">
-    <cfRule type="expression" dxfId="8" priority="357">
+    <cfRule type="expression" dxfId="9" priority="357">
       <formula>AND(CM$5&gt;=#REF!,CM$5&lt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CM32:CO32">
-    <cfRule type="expression" dxfId="7" priority="358">
+  <conditionalFormatting sqref="CM32:CO32 CM53:CO54">
+    <cfRule type="expression" dxfId="8" priority="358">
       <formula>AND(CM$5&gt;=$B34,CM$5&lt;=$C34)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CM34:CO34">
-    <cfRule type="expression" dxfId="6" priority="360">
+    <cfRule type="expression" dxfId="7" priority="360">
       <formula>AND(CM$5&gt;=$B41,CM$5&lt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33:EG33">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>D$5=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>D$5=$C$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33:EG33">
-    <cfRule type="expression" dxfId="3" priority="8">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>AND(D$5&gt;=$B33,D$5&lt;=$C33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33:EG33">
-    <cfRule type="expression" dxfId="2" priority="9">
+    <cfRule type="expression" dxfId="3" priority="9">
       <formula>AND(D$5&gt;=#REF!,D$5&lt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CM44:CO44">
-    <cfRule type="expression" dxfId="1" priority="374">
+    <cfRule type="expression" dxfId="2" priority="374">
       <formula>AND(CM$5&gt;=$B42,CM$5&lt;=$C42)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CM44:CO44">
-    <cfRule type="expression" dxfId="0" priority="376">
+    <cfRule type="expression" dxfId="1" priority="376">
       <formula>AND(CM$5&gt;=$B49,CM$5&lt;=#REF!)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CM46:CO54">
+    <cfRule type="expression" dxfId="0" priority="382">
+      <formula>AND(CM$5&gt;=$B55,CM$5&lt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>